<commit_message>
local variable global variable supermarket
</commit_message>
<xml_diff>
--- a/HomeworkScore.xlsx
+++ b/HomeworkScore.xlsx
@@ -293,13 +293,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>409020</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>75648</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -617,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U77"/>
+  <dimension ref="A1:U78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18"/>
@@ -1021,7 +1021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:9">
       <c r="A17" s="2">
         <v>44142</v>
       </c>
@@ -1042,7 +1042,7 @@
       </c>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:9">
       <c r="A18" s="2">
         <v>44149</v>
       </c>
@@ -1063,228 +1063,251 @@
       </c>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:21" s="1" customFormat="1">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:9">
+      <c r="A19" s="2">
+        <v>44156</v>
+      </c>
+      <c r="B19" s="3">
+        <v>20</v>
+      </c>
+      <c r="C19" s="3">
+        <v>20</v>
+      </c>
+      <c r="D19" s="3">
+        <v>20</v>
+      </c>
+      <c r="E19" s="3">
+        <v>20</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3">
+        <v>20</v>
+      </c>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" s="1" customFormat="1">
+      <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="3">
-        <f>SUM(B2:B18)</f>
-        <v>250</v>
-      </c>
-      <c r="C19" s="3">
-        <f>SUM(C2:C18)</f>
-        <v>160</v>
-      </c>
-      <c r="D19" s="3">
+      <c r="B20" s="3">
+        <f>SUM(B2:B19)</f>
+        <v>270</v>
+      </c>
+      <c r="C20" s="3">
+        <f>SUM(C2:C19)</f>
+        <v>180</v>
+      </c>
+      <c r="D20" s="3">
         <f>SUM(D2:D13)</f>
         <v>40</v>
       </c>
-      <c r="E19" s="3">
-        <f>SUM(E2:E18)</f>
-        <v>150</v>
-      </c>
-      <c r="F19" s="3">
+      <c r="E20" s="3">
+        <f>SUM(E2:E19)</f>
+        <v>170</v>
+      </c>
+      <c r="F20" s="3">
         <f>SUM(F2:F16)</f>
         <v>180</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G20" s="3">
         <f>SUM(G2:G16)</f>
         <v>150</v>
       </c>
-      <c r="H19" s="3">
-        <f>SUM(H2:H18)</f>
-        <v>250</v>
-      </c>
-      <c r="I19" s="3">
-        <f t="shared" ref="I19" si="0">SUM(I2:I13)</f>
+      <c r="H20" s="3">
+        <f>SUM(H2:H19)</f>
+        <v>270</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" ref="I20" si="0">SUM(I2:I13)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
-      <c r="A20" s="3" t="s">
+    <row r="21" spans="1:9">
+      <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B21" s="3">
         <v>100</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C21" s="3">
         <v>100</v>
       </c>
-      <c r="D20" s="3">
-        <v>0</v>
-      </c>
-      <c r="E20" s="3">
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
         <v>100</v>
       </c>
-      <c r="F20" s="3">
-        <v>0</v>
-      </c>
-      <c r="G20" s="3">
-        <v>0</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
-      <c r="A21" s="3" t="s">
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0</v>
+      </c>
+      <c r="H21" s="3">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="3">
-        <f>B19-B20</f>
-        <v>150</v>
-      </c>
-      <c r="C21" s="3">
-        <f t="shared" ref="C21:I21" si="1">C19-C20</f>
-        <v>60</v>
-      </c>
-      <c r="D21" s="3">
-        <f>D19-D20</f>
+      <c r="B22" s="3">
+        <f>B20-B21</f>
+        <v>170</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" ref="C22:I22" si="1">C20-C21</f>
+        <v>80</v>
+      </c>
+      <c r="D22" s="3">
+        <f>D20-D21</f>
         <v>40</v>
       </c>
-      <c r="E21" s="3">
-        <f>E19-E20</f>
-        <v>50</v>
-      </c>
-      <c r="F21" s="3">
+      <c r="E22" s="3">
+        <f>E20-E21</f>
+        <v>70</v>
+      </c>
+      <c r="F22" s="3">
         <f t="shared" si="1"/>
         <v>180</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G22" s="3">
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H22" s="3">
         <f t="shared" si="1"/>
-        <v>250</v>
-      </c>
-      <c r="I21" s="3">
+        <v>270</v>
+      </c>
+      <c r="I22" s="3">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
-      <c r="A26" s="4" t="s">
+    <row r="27" spans="1:9">
+      <c r="A27" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
-      <c r="A27" s="2">
-        <v>44087</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="3">
-        <v>100</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="F27" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:9">
       <c r="A28" s="2">
         <v>44087</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C28" s="3">
         <v>100</v>
       </c>
+      <c r="D28" s="7"/>
       <c r="F28" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="3">
+        <v>100</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
-      <c r="F29" s="2" t="s">
+    <row r="30" spans="1:9">
+      <c r="F30" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
-      <c r="F30" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21">
+    <row r="31" spans="1:9">
       <c r="F31" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="F32" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
-      <c r="A32" s="2">
+    <row r="33" spans="1:21">
+      <c r="A33" s="2">
         <v>44128</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C33" s="3">
         <v>100</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F33" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="U32" s="2" t="s">
+      <c r="U33" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="6:6">
-      <c r="F33" s="2" t="s">
+    <row r="34" spans="1:21">
+      <c r="F34" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="6:6">
-      <c r="F41" s="1" t="s">
+    <row r="42" spans="1:21">
+      <c r="F42" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="53" spans="5:8">
-      <c r="E53" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G53" s="7"/>
-      <c r="H53" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="54" spans="5:8">
       <c r="E54" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G54" s="7"/>
+      <c r="H54" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="5:8">
+      <c r="E55" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G54" s="7"/>
-      <c r="H54" s="8" t="s">
+      <c r="G55" s="7"/>
+      <c r="H55" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="5:8">
-      <c r="H55" s="1" t="s">
+    <row r="56" spans="5:8">
+      <c r="H56" s="1" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="76" spans="5:8">
-      <c r="E76" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H76" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="77" spans="5:8">
       <c r="E77" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="78" spans="5:8">
+      <c r="E78" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H77" s="1" t="s">
+      <c r="H78" s="1" t="s">
         <v>35</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H54" r:id="rId1"/>
+    <hyperlink ref="H55" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>